<commit_message>
Home Work Lesson3 Release
</commit_message>
<xml_diff>
--- a/Mathematics/Lesson3/FMLesson3.xlsx
+++ b/Mathematics/Lesson3/FMLesson3.xlsx
@@ -213,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -252,6 +252,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
@@ -756,16 +757,16 @@
         <v>15</v>
       </c>
       <c r="B12" s="16">
-        <f>H6</f>
-        <v>1.432312839</v>
+        <f>H7</f>
+        <v>0.05266728586</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="16">
-        <f>STDEVA(B4:H4)</f>
+      <c r="B13" s="17">
+        <f>STDEVA(B5:H5)</f>
         <v>0.06241184259</v>
       </c>
     </row>
@@ -773,9 +774,9 @@
       <c r="A14" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="17">
         <f>B12/B13</f>
-        <v>22.94937595</v>
+        <v>0.8438668637</v>
       </c>
     </row>
   </sheetData>
@@ -822,7 +823,7 @@
       <c r="A7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="18">
         <v>0.3</v>
       </c>
     </row>
@@ -830,7 +831,7 @@
       <c r="A8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="18">
         <v>0.01</v>
       </c>
     </row>
@@ -838,7 +839,7 @@
       <c r="A9" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="19">
         <f>30%*1%+50%*3%+20%*10%</f>
         <v>0.038</v>
       </c>
@@ -852,7 +853,7 @@
       <c r="A11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="20">
         <f>B8*B7/B9</f>
         <v>0.07894736842</v>
       </c>
@@ -984,9 +985,9 @@
       <c r="M8" s="9">
         <v>16.9</v>
       </c>
-      <c r="N8" s="20">
+      <c r="N8" s="21">
         <f>B12*N9+C12</f>
-        <v>17.79519621</v>
+        <v>17.19749019</v>
       </c>
     </row>
     <row r="9">
@@ -1030,14 +1031,14 @@
         <v>159.0</v>
       </c>
       <c r="N9" s="9">
-        <v>180.0</v>
+        <v>173.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="17">
         <f>CORREL(B8:M8,B9:M9)</f>
         <v>0.8474507018</v>
       </c>
@@ -1046,12 +1047,12 @@
       <c r="A12" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="16">
-        <f t="array" ref="B12:C12">LINEST(B8:M8,B9:M9)</f>
-        <v>0.05541322117</v>
-      </c>
-      <c r="C12" s="16">
-        <v>7.82081640456957</v>
+      <c r="B12" s="17">
+        <f t="array" ref="B12:C12">LINEST(C8:M8,B9:L9)</f>
+        <v>0.03313482782</v>
+      </c>
+      <c r="C12" s="17">
+        <v>11.465164981468813</v>
       </c>
     </row>
   </sheetData>

</xml_diff>